<commit_message>
try clone in other laptop
</commit_message>
<xml_diff>
--- a/CAMERA_DATA_LABELS_2020-08-13_1400.xlsx
+++ b/CAMERA_DATA_LABELS_2020-08-13_1400.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sibas\Google Drive Streaming\My Drive\UBC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sibas\Google Drive Streaming\My Drive\UBC\Codes\fusion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:8001_{62FB2FE9-7EE8-4BFB-BB2A-EAB9A4601BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A7F6BE-9786-423F-B80F-22615E05EEC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CAMERA_DATA_LABELS_2020-08-13_1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1699" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1697" uniqueCount="139">
   <si>
     <t>Study ID</t>
   </si>
@@ -437,9 +437,6 @@
   </si>
   <si>
     <t>folder</t>
-  </si>
-  <si>
-    <t>9339 - 9629</t>
   </si>
 </sst>
 </file>
@@ -1258,8 +1255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BU53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3790,10 +3787,10 @@
         <v>1015</v>
       </c>
       <c r="B16">
-        <v>9525</v>
+        <v>9351</v>
       </c>
       <c r="C16">
-        <v>20200127</v>
+        <v>20200227</v>
       </c>
       <c r="E16" t="s">
         <v>71</v>
@@ -5865,8 +5862,8 @@
       <c r="A28">
         <v>1027</v>
       </c>
-      <c r="B28" t="s">
-        <v>139</v>
+      <c r="B28">
+        <v>9629</v>
       </c>
       <c r="C28">
         <v>20200206</v>
@@ -6050,8 +6047,8 @@
       <c r="A29">
         <v>1028</v>
       </c>
-      <c r="B29" t="s">
-        <v>139</v>
+      <c r="B29">
+        <v>9339</v>
       </c>
       <c r="C29">
         <v>20200206</v>

</xml_diff>